<commit_message>
Improved comparison logic for Excel and CSV files:
- Updated the file reading logic to clean headers while preserving key characters for precise comparisons.
- Enhanced the comparison algorithm to ensure distinct values like 'AlXexander_xyz' and 'Alexander' are properly differentiated.
- Added support for both Excel and CSV file uploads with consistent header cleaning across both formats.
- Improved column mapping interface for a more intuitive user experience.
- Ensured that lazy loading and async handling are implemented for smoother user interaction with large datasets.
</commit_message>
<xml_diff>
--- a/assets/data/vergleich.xlsx
+++ b/assets/data/vergleich.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/louisstark/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/louisstark/Documents/IntelliJ_Projects/file-compare/assets/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5CF72153-F50E-EA4E-AE14-473937E5EC30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C01AA4-C08F-3D4E-AE1E-B123840863B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10860" yWindow="6620" windowWidth="27640" windowHeight="16940" xr2:uid="{8B9FAF44-1AC4-B240-B9DB-F844C28BB52D}"/>
   </bookViews>
@@ -37,18 +37,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Alter</t>
   </si>
   <si>
-    <t>Stadt</t>
-  </si>
-  <si>
     <t>Clara</t>
   </si>
   <si>
@@ -107,6 +98,15 @@
   </si>
   <si>
     <t>Erfurt</t>
+  </si>
+  <si>
+    <t>KundenNummer</t>
+  </si>
+  <si>
+    <t>Vorname</t>
+  </si>
+  <si>
+    <t>Ort</t>
   </si>
 </sst>
 </file>
@@ -474,23 +474,23 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A11"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:4" ht="17">
       <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17">
@@ -498,13 +498,13 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17">
@@ -512,13 +512,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17">
@@ -526,13 +526,13 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17">
@@ -540,13 +540,13 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17">
@@ -554,13 +554,13 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C6">
         <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17">
@@ -568,13 +568,13 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C7">
         <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17">
@@ -582,13 +582,13 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C8">
         <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17">
@@ -596,13 +596,13 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C9">
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17">
@@ -610,13 +610,13 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C10">
         <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17">
@@ -624,13 +624,13 @@
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C11">
         <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>